<commit_message>
Add enemy dead animation
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fish/Documents/FYP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fish/Projects/FYP/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -218,6 +218,22 @@
   </si>
   <si>
     <t>In progress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unusual Attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy will damage by player without player attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -544,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -792,10 +808,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -873,6 +889,23 @@
         <v>43100</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="1">
+        <v>43104</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H2"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
village screen is finished
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fish/Projects/FYP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fish/Documents/FYP/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -213,39 +213,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Unusual Attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enemy will damage by player without player attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Forest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Fish</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Kuen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>In progress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Player pass through terrain</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fish</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fish</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -573,7 +545,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -660,14 +632,8 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
-        <v>53</v>
-      </c>
       <c r="F4" s="1">
         <v>43096</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -694,8 +660,14 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
       <c r="F6" s="1">
         <v>43100</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -742,14 +714,8 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" t="s">
-        <v>49</v>
-      </c>
       <c r="F9" s="1">
         <v>43100</v>
-      </c>
-      <c r="H9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
@@ -826,15 +792,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -907,34 +873,6 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="1">
-        <v>43104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:H2"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
try to fix the spider attack after dead, but not succes
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fish/Projects/FYP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cckhh\Documents\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="1128" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -19,10 +19,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Defect!$A$1:$H$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Todo '!$A$1:$H$4</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -311,24 +311,42 @@
   <si>
     <t>Fish</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy attack</t>
+  </si>
+  <si>
+    <t>Enemy could still attack once after its dead. It leads to the level up times cut to once only</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>All UI item should be private</t>
+  </si>
+  <si>
+    <t>7jan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -356,16 +374,19 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -634,24 +655,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -667,17 +688,17 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -690,14 +711,14 @@
       <c r="E2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="1">
-        <v>43103</v>
+      <c r="F2" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -707,11 +728,11 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F3" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -724,17 +745,17 @@
       <c r="E4" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="1">
-        <v>43103</v>
-      </c>
-      <c r="G4" s="1">
-        <v>43107</v>
+      <c r="F4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -747,14 +768,14 @@
       <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="1">
-        <v>43103</v>
+      <c r="F5" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -764,14 +785,14 @@
       <c r="E6" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="1">
-        <v>43103</v>
+      <c r="F6" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -781,11 +802,11 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F7" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -795,11 +816,11 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F8" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -809,28 +830,28 @@
       <c r="E9" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="1">
-        <v>43103</v>
-      </c>
-      <c r="G9" s="1">
-        <v>43106</v>
+      <c r="F9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F10" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -846,17 +867,17 @@
       <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="1">
-        <v>43103</v>
-      </c>
-      <c r="G11" s="1">
-        <v>43106</v>
+      <c r="F11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -869,156 +890,169 @@
       <c r="E12" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="1">
-        <v>43103</v>
+      <c r="F12" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>33</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F13" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>47</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F14" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>54</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F15" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>55</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>57</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F17" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>58</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F18" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>59</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F19" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>63</v>
       </c>
       <c r="D20" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F20" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>65</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F21" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>66</v>
       </c>
       <c r="D22" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="1">
-        <v>43103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F22" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>68</v>
       </c>
       <c r="D23" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="1">
-        <v>43103</v>
+      <c r="F23" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H4"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1034,17 +1068,17 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1060,17 +1094,17 @@
       <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="1">
-        <v>43096</v>
-      </c>
-      <c r="G2" s="1">
-        <v>43103</v>
+      <c r="F2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1083,11 +1117,11 @@
       <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="1">
-        <v>43100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F3" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1100,11 +1134,11 @@
       <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="1">
-        <v>43104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F4" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1113,6 +1147,26 @@
       </c>
       <c r="D5" t="s">
         <v>45</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cut attack animation and disable moving when attack
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cckhh\Documents\FYP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fish/Projects/FYP/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1128" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Defect!$A$1:$H$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Todo '!$A$1:$H$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Todo '!$A$1:$H$26</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -237,10 +237,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UI - skill and menu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Kuen</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -273,11 +269,82 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Kit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item drop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System menu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy attack</t>
+  </si>
+  <si>
+    <t>Enemy could still attack once after its dead. It leads to the level up times cut to once only</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>All UI item should be private</t>
+  </si>
+  <si>
+    <t>Up level animation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 Jan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 Jan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>In progress</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Kit</t>
+    <t>Harry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In progress</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -285,68 +352,58 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Classes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fish</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item drop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fish</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System menu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fish</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enemy attack</t>
-  </si>
-  <si>
-    <t>Enemy could still attack once after its dead. It leads to the level up times cut to once only</t>
-  </si>
-  <si>
-    <t>Forest</t>
-  </si>
-  <si>
-    <t>Fish</t>
-  </si>
-  <si>
-    <t>All UI item should be private</t>
-  </si>
-  <si>
-    <t>7jan</t>
+    <t>7 Jan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pending</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player Attribute - UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buff - UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11 Jan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -377,7 +434,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -655,24 +712,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -698,7 +756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -712,13 +770,13 @@
         <v>37</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -728,11 +786,20 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>74</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -746,16 +813,16 @@
         <v>46</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -769,30 +836,33 @@
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>75</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>51</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -802,11 +872,20 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>74</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -816,11 +895,17 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>74</v>
+      </c>
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -831,16 +916,16 @@
         <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -848,10 +933,10 @@
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -868,16 +953,16 @@
         <v>36</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -888,16 +973,16 @@
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -905,10 +990,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -916,121 +1001,169 @@
         <v>5</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
         <v>54</v>
       </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
         <v>57</v>
       </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
         <v>63</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
+      <c r="D23" t="s">
         <v>65</v>
       </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
+      <c r="F23" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
         <v>66</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="F24" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>75</v>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H4"/>
+  <autoFilter ref="A1:H26">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="In progress"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1041,18 +1174,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="D19:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.19921875" style="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1078,7 +1211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1095,16 +1228,16 @@
         <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1118,10 +1251,10 @@
         <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1135,10 +1268,10 @@
         <v>42</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1149,24 +1282,24 @@
         <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
         <v>70</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add player attribute ui
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="92">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -389,6 +389,10 @@
   </si>
   <si>
     <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In progress</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -743,7 +747,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1056,10 +1060,13 @@
         <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>74</v>
+      </c>
+      <c r="H16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
hp and mp bar text
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fish/Projects/FYP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cckhh\Documents\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="2256" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="95">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -394,24 +394,33 @@
   <si>
     <t>In progress</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>min damage 1</t>
+  </si>
+  <si>
+    <t>14 Jan</t>
+  </si>
+  <si>
+    <t>db and save</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -442,7 +451,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -744,24 +753,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -787,7 +796,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -807,7 +816,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -830,7 +839,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -853,7 +862,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -876,7 +885,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -893,7 +902,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -916,7 +925,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -936,7 +945,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -956,7 +965,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -967,7 +976,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -993,7 +1002,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1013,7 +1022,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1024,7 +1033,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1052,7 +1061,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1086,7 +1095,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1097,7 +1106,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -1108,7 +1117,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1119,7 +1128,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1130,7 +1139,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1141,7 +1150,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1152,7 +1161,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -1163,7 +1172,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1174,7 +1183,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -1185,7 +1194,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -1194,6 +1203,31 @@
       </c>
       <c r="F27" s="1" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1214,14 +1248,14 @@
       <selection activeCell="E19" sqref="D19:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.1640625" style="1"/>
+    <col min="1" max="1" width="21.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1247,7 +1281,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1273,7 +1307,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1290,7 +1324,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1307,7 +1341,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1321,7 +1355,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
add cd and gcd  to todo
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500"/>
+    <workbookView xWindow="4512" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="101">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -412,6 +412,15 @@
   </si>
   <si>
     <t>add a super algo to cal the 1 damage</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>gcd</t>
+  </si>
+  <si>
+    <t>fish</t>
   </si>
 </sst>
 </file>
@@ -762,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1249,6 +1258,28 @@
       </c>
       <c r="E29" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add save load script
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="108">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -432,6 +432,22 @@
   </si>
   <si>
     <t>Complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refactor code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refactor the code not done by ourselves</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 Jan</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -783,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1283,7 +1299,7 @@
         <v>96</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E30" t="s">
         <v>98</v>
@@ -1297,13 +1313,27 @@
         <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s">
         <v>98</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update todo list and player attribute script
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
     <sheet name="Defect" sheetId="2" r:id="rId2"/>
+    <sheet name="Remark" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Defect!$A$1:$H$2</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="126">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -464,6 +465,62 @@
   </si>
   <si>
     <t>In progress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adjust camera</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 Jan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migreate light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 Jan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Log console</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 Jan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weapon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 - 199</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 - 99</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Armor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200 - 299</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -819,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1377,6 +1434,42 @@
       </c>
       <c r="H33" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1526,4 +1619,44 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add loading screen when load and save
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="131">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -521,6 +521,26 @@
   </si>
   <si>
     <t>200 - 299</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player attack cd missing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21 Jan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solved</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1484,16 +1504,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="D19:E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
@@ -1565,6 +1585,12 @@
       <c r="F3" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
@@ -1612,6 +1638,17 @@
       </c>
       <c r="F6" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1625,7 +1662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish the equipment system
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fish/Projects/FYP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cckhh\Documents\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="1116" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="166">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -666,23 +666,35 @@
     <t>6 Feb</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Save Object</t>
+  </si>
+  <si>
+    <t>Can't save object if the bag has not been enabled.</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>10 Mar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -696,7 +708,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -736,8 +748,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1041,22 +1053,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1082,7 +1094,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1105,7 +1117,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1128,7 +1140,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1151,7 +1163,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1174,7 +1186,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1194,7 +1206,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1217,7 +1229,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1240,7 +1252,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1260,7 +1272,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1271,7 +1283,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1297,7 +1309,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1317,7 +1329,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1328,7 +1340,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1339,7 +1351,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1356,7 +1368,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1373,7 +1385,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1390,7 +1402,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -1401,7 +1413,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1412,7 +1424,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1423,7 +1435,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1434,7 +1446,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1445,7 +1457,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1456,7 +1468,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -1467,7 +1479,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1478,7 +1490,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -1489,7 +1501,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1500,7 +1512,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>89</v>
       </c>
@@ -1523,7 +1535,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -1540,7 +1552,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -1554,7 +1566,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>96</v>
       </c>
@@ -1568,7 +1580,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>155</v>
       </c>
@@ -1579,7 +1591,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -1599,7 +1611,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>111</v>
       </c>
@@ -1610,7 +1622,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>126</v>
       </c>
@@ -1624,7 +1636,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -1635,7 +1647,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>127</v>
       </c>
@@ -1652,7 +1664,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>129</v>
       </c>
@@ -1663,7 +1675,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -1677,7 +1689,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -1691,7 +1703,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8">
       <c r="A41" s="2" t="s">
         <v>136</v>
       </c>
@@ -1702,7 +1714,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
         <v>137</v>
       </c>
@@ -1713,7 +1725,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
         <v>138</v>
       </c>
@@ -1724,7 +1736,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
         <v>139</v>
       </c>
@@ -1738,7 +1750,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>142</v>
       </c>
@@ -1752,7 +1764,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>143</v>
       </c>
@@ -1766,7 +1778,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
         <v>145</v>
       </c>
@@ -1780,7 +1792,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
         <v>147</v>
       </c>
@@ -1794,7 +1806,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>149</v>
       </c>
@@ -1808,7 +1820,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>151</v>
       </c>
@@ -1819,7 +1831,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>153</v>
       </c>
@@ -1852,20 +1864,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.1640625" style="1"/>
+    <col min="1" max="1" width="21.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1891,7 +1903,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1917,7 +1929,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1940,7 +1952,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1957,7 +1969,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1971,7 +1983,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1986,6 +1998,23 @@
       </c>
       <c r="F6" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2003,9 +2032,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -2013,7 +2042,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -2021,7 +2050,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
could new a character and load to village,ui but cant unload the newcharacter due to the start of loadscenemanager and saveobject
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2232" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="170">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -677,6 +677,18 @@
   </si>
   <si>
     <t>10 Mar</t>
+  </si>
+  <si>
+    <t>new char texture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the char in new char are so shinnydue to the texture in new char is modified by ghost </t>
+  </si>
+  <si>
+    <t>NewCharacter</t>
+  </si>
+  <si>
+    <t>30 Mar</t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1864,10 +1876,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A8" sqref="A8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2015,6 +2027,26 @@
       </c>
       <c r="F7" s="1" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ng chi gay si do der
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3350" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="4470" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="178">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -698,6 +698,21 @@
   </si>
   <si>
     <t>02 Apr</t>
+  </si>
+  <si>
+    <t>loading bar</t>
+  </si>
+  <si>
+    <t>loading for scene changing</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>ui</t>
+  </si>
+  <si>
+    <t>mute at setting and staating page</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5"/>
@@ -1873,6 +1888,9 @@
       <c r="B52" t="s">
         <v>171</v>
       </c>
+      <c r="C52" t="s">
+        <v>176</v>
+      </c>
       <c r="D52" t="s">
         <v>70</v>
       </c>
@@ -1880,6 +1898,43 @@
         <v>70</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" t="s">
+        <v>174</v>
+      </c>
+      <c r="C53" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" t="s">
+        <v>70</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" t="s">
+        <v>175</v>
+      </c>
+      <c r="D54" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add the id and unit for equipment
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="5592" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="181">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -496,23 +496,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Weapon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 - 199</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0 - 99</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Armor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>200 - 299</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -713,6 +697,27 @@
   </si>
   <si>
     <t>mute at setting and staating page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equipment </t>
+  </si>
+  <si>
+    <t>100-199</t>
+  </si>
+  <si>
+    <t>boot 141</t>
+  </si>
+  <si>
+    <t>bracer 131</t>
+  </si>
+  <si>
+    <t>breast 121</t>
+  </si>
+  <si>
+    <t>weapon 111</t>
+  </si>
+  <si>
+    <t>cap 101</t>
   </si>
 </sst>
 </file>
@@ -1089,18 +1094,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1147,10 +1152,10 @@
         <v>73</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1412,7 +1417,7 @@
         <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>73</v>
@@ -1618,13 +1623,13 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1660,7 +1665,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C35" t="s">
         <v>114</v>
@@ -1685,7 +1690,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D37" t="s">
         <v>5</v>
@@ -1694,35 +1699,35 @@
         <v>32</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H37" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D38" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1741,155 +1746,155 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D41" t="s">
         <v>80</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D42" t="s">
         <v>80</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D43" t="s">
         <v>80</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D44" t="s">
         <v>80</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D45" t="s">
         <v>80</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D46" t="s">
         <v>80</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D47" t="s">
         <v>80</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D48" t="s">
         <v>80</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D49" t="s">
         <v>80</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D50" t="s">
         <v>80</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D51" t="s">
         <v>80</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C52" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D52" t="s">
         <v>70</v>
@@ -1898,18 +1903,18 @@
         <v>70</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B53" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C53" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D53" t="s">
         <v>70</v>
@@ -1918,15 +1923,15 @@
         <v>70</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C54" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D54" t="s">
         <v>70</v>
@@ -1935,7 +1940,7 @@
         <v>70</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1963,11 +1968,11 @@
       <selection activeCell="A8" sqref="A8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.1640625" style="1"/>
+    <col min="1" max="1" width="21.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.19921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2039,10 +2044,10 @@
         <v>73</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2095,30 +2100,30 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D7" t="s">
         <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D8" t="s">
         <v>70</v>
@@ -2127,7 +2132,7 @@
         <v>70</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2139,36 +2144,49 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" t="s">
-        <v>123</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="E5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="D6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="E7" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update exp formula, add color to in game log
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fish/Projects/FYP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cckhh\Documents\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1116" yWindow="456" windowWidth="25596" windowHeight="15456" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Todo " sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="188">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -735,23 +735,32 @@
     <t>Complete</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>cant set main cam after create</t>
+  </si>
+  <si>
+    <t>double click thecreate could produce the bug</t>
+  </si>
+  <si>
+    <t>12 Apr</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -765,7 +774,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -805,8 +814,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1114,18 +1123,18 @@
       <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +1160,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1174,7 +1183,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1197,7 +1206,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1220,7 +1229,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1243,7 +1252,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1263,7 +1272,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1286,7 +1295,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1309,7 +1318,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1329,7 +1338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1340,7 +1349,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1366,7 +1375,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1386,7 +1395,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1397,7 +1406,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1408,7 +1417,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1425,7 +1434,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1442,7 +1451,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1459,7 +1468,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -1470,7 +1479,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1481,7 +1490,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1492,7 +1501,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1503,7 +1512,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1514,7 +1523,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1525,7 +1534,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -1536,7 +1545,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1547,7 +1556,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -1561,7 +1570,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1572,7 +1581,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -1595,7 +1604,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -1612,7 +1621,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>94</v>
       </c>
@@ -1626,7 +1635,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -1640,7 +1649,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>150</v>
       </c>
@@ -1651,7 +1660,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -1671,7 +1680,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -1682,7 +1691,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -1696,7 +1705,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>116</v>
       </c>
@@ -1707,7 +1716,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>122</v>
       </c>
@@ -1724,7 +1733,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>124</v>
       </c>
@@ -1738,7 +1747,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>127</v>
       </c>
@@ -1752,7 +1761,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -1766,7 +1775,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8">
       <c r="A41" s="2" t="s">
         <v>131</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
         <v>132</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
         <v>133</v>
       </c>
@@ -1799,7 +1808,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
         <v>134</v>
       </c>
@@ -1813,7 +1822,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>137</v>
       </c>
@@ -1827,7 +1836,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>138</v>
       </c>
@@ -1841,7 +1850,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
         <v>140</v>
       </c>
@@ -1855,7 +1864,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
         <v>142</v>
       </c>
@@ -1869,7 +1878,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -1883,7 +1892,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>146</v>
       </c>
@@ -1894,7 +1903,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>148</v>
       </c>
@@ -1908,7 +1917,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>164</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>167</v>
       </c>
@@ -1948,7 +1957,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>171</v>
       </c>
@@ -1984,20 +1993,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.1640625" style="1"/>
+    <col min="1" max="1" width="21.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2023,7 +2032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2049,7 +2058,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2072,7 +2081,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -2089,7 +2098,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -2103,7 +2112,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -2120,7 +2129,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>156</v>
       </c>
@@ -2137,7 +2146,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>160</v>
       </c>
@@ -2155,6 +2164,26 @@
       </c>
       <c r="F8" s="1" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2172,9 +2201,9 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -2182,7 +2211,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>172</v>
       </c>
@@ -2190,12 +2219,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6">
       <c r="E5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6">
       <c r="D6" t="s">
         <v>177</v>
       </c>
@@ -2206,7 +2235,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6">
       <c r="E7" t="s">
         <v>174</v>
       </c>

</xml_diff>